<commit_message>
adding str.format to prac3, adding metadata file
</commit_message>
<xml_diff>
--- a/Data/LSOA_metadata.xlsx
+++ b/Data/LSOA_metadata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1076631\Google Drive\repos\geocomputation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1076631\Google Drive\repos\geocomputation (1)\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="8040" xr2:uid="{593C3E9E-18B4-479B-90C3-43D8609D58BF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="8040" activeTab="1" xr2:uid="{593C3E9E-18B4-479B-90C3-43D8609D58BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="164">
   <si>
     <t>LSOA11CD</t>
   </si>
@@ -385,6 +385,138 @@
   </si>
   <si>
     <t>SharedOwnshp</t>
+  </si>
+  <si>
+    <t>microgrammes per metre cubed</t>
+  </si>
+  <si>
+    <t>London Data Store Pollution</t>
+  </si>
+  <si>
+    <t>Mean of 20m pixels (each of which are annual NO2) in the LSOA</t>
+  </si>
+  <si>
+    <t>Mean of 20m pixels (each of which are annual PM10) in the LSOA</t>
+  </si>
+  <si>
+    <t>Standard Deviation of 20m pixels (each of which are annual NO2) in the LSOA</t>
+  </si>
+  <si>
+    <t>Standard Deviation of 20m pixels (each of which are annual NOx) in the LSOA</t>
+  </si>
+  <si>
+    <t>Standard Deviation of 20m pixels (each of which are annual PM10) in the LSOA</t>
+  </si>
+  <si>
+    <t>Maximum value of 20m pixels (each of which are annual NO2) in the LSOA</t>
+  </si>
+  <si>
+    <t>Minimum value of 20m pixels (each of which are annual NO2) in the LSOA</t>
+  </si>
+  <si>
+    <t>Maximum value of 20m pixels (each of which are annual NOx) in the LSOA</t>
+  </si>
+  <si>
+    <t>Minimum value of 20m pixels (each of which are annual NOx) in the LSOA</t>
+  </si>
+  <si>
+    <t>Mean of 20m pixels (each of which are annual NOx) in the LSOA</t>
+  </si>
+  <si>
+    <t>Maximum value of 20m pixels (each of which are annual PM10) in the LSOA</t>
+  </si>
+  <si>
+    <t>Minimum value of 20m pixels (each of which are annual PM10) in the LSOA</t>
+  </si>
+  <si>
+    <t>Standard Deviation of 20m pixels (each of which are annual PM2.5) in the LSOA</t>
+  </si>
+  <si>
+    <t>Maximum value of 20m pixels (each of which are annual PM2.5) in the LSOA</t>
+  </si>
+  <si>
+    <t>Minimum value of 20m pixels (each of which are annual PM2.5) in the LSOA</t>
+  </si>
+  <si>
+    <t>Mean of 20m pixels (each of which are annual PM2.5) in the LSOA</t>
+  </si>
+  <si>
+    <t>Area of LSOA</t>
+  </si>
+  <si>
+    <t>Population Density</t>
+  </si>
+  <si>
+    <t>Households</t>
+  </si>
+  <si>
+    <t>Mean persons per household</t>
+  </si>
+  <si>
+    <t>Usual residents</t>
+  </si>
+  <si>
+    <t>Households residents</t>
+  </si>
+  <si>
+    <t>Geometry of shapefile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://data.london.gov.uk/dataset/london-atmospheric-emissions-inventory-2013 </t>
+  </si>
+  <si>
+    <t>Mixed/multiple ethnic groups, Ethnicity from 2011 Census</t>
+  </si>
+  <si>
+    <t>White. Ethnicity from 2011 Census</t>
+  </si>
+  <si>
+    <t>Asian/Asian British, Ethnicity from 2011 Census</t>
+  </si>
+  <si>
+    <t>Black/African/Caribbean/Black British, Ethnicity from 2011 Census</t>
+  </si>
+  <si>
+    <t>Other ethnic group, Ethnicity from 2011 Census</t>
+  </si>
+  <si>
+    <t>Living rent free, Tenure of household from 2011 census</t>
+  </si>
+  <si>
+    <t>Private rented, Tenure of household from 2011 census</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ons.gov.uk/census/2011census/2011censusdata/2011censususerguide/variablesandclassifications </t>
+  </si>
+  <si>
+    <t>Link3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ons.gov.uk/census/2011census/2011censusdata/2011censususerguide/glossary </t>
+  </si>
+  <si>
+    <t>Average number of bedrooms per household, from 2011 census</t>
+  </si>
+  <si>
+    <t>Average number of rooms per household, from 2011 census</t>
+  </si>
+  <si>
+    <t>Occupancy rating (bedrooms) of -1 or less, from 2011 census</t>
+  </si>
+  <si>
+    <t>Occupancy rating (rooms) of -1 or less, from 2011 census</t>
+  </si>
+  <si>
+    <t>Social rented, Tenure of household from 2011 census</t>
+  </si>
+  <si>
+    <t>Owned, Tenure of household from 2011 census</t>
+  </si>
+  <si>
+    <t>Shared ownership (part owned and part rented), Tenure of household from 2011 census</t>
+  </si>
+  <si>
+    <t>Accomodation type</t>
   </si>
 </sst>
 </file>
@@ -758,15 +890,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308D1A97-3E7F-4F8B-8A8D-3559D0C42BFD}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -961,6 +1093,9 @@
       <c r="C10" t="s">
         <v>44</v>
       </c>
+      <c r="D10" t="s">
+        <v>142</v>
+      </c>
       <c r="E10" t="s">
         <v>55</v>
       </c>
@@ -978,6 +1113,9 @@
       <c r="C11" t="s">
         <v>44</v>
       </c>
+      <c r="D11" t="s">
+        <v>143</v>
+      </c>
       <c r="E11" t="s">
         <v>55</v>
       </c>
@@ -1015,6 +1153,9 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
+      <c r="D13" t="s">
+        <v>139</v>
+      </c>
       <c r="E13" t="s">
         <v>59</v>
       </c>
@@ -1032,6 +1173,9 @@
       <c r="C14" t="s">
         <v>44</v>
       </c>
+      <c r="D14" t="s">
+        <v>140</v>
+      </c>
       <c r="E14" t="s">
         <v>54</v>
       </c>
@@ -1049,6 +1193,9 @@
       <c r="C15" t="s">
         <v>44</v>
       </c>
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
       <c r="E15" t="s">
         <v>58</v>
       </c>
@@ -1066,6 +1213,9 @@
       <c r="C16" t="s">
         <v>44</v>
       </c>
+      <c r="D16" t="s">
+        <v>144</v>
+      </c>
       <c r="E16" t="s">
         <v>57</v>
       </c>
@@ -1083,6 +1233,9 @@
       <c r="C17" t="s">
         <v>46</v>
       </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
       <c r="E17" t="s">
         <v>94</v>
       </c>
@@ -1100,6 +1253,9 @@
       <c r="C18" t="s">
         <v>47</v>
       </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
       <c r="E18" t="s">
         <v>94</v>
       </c>
@@ -1117,6 +1273,9 @@
       <c r="C19" t="s">
         <v>48</v>
       </c>
+      <c r="D19" t="s">
+        <v>161</v>
+      </c>
       <c r="E19" t="s">
         <v>54</v>
       </c>
@@ -1134,6 +1293,9 @@
       <c r="C20" t="s">
         <v>48</v>
       </c>
+      <c r="D20" t="s">
+        <v>162</v>
+      </c>
       <c r="E20" t="s">
         <v>54</v>
       </c>
@@ -1151,6 +1313,9 @@
       <c r="C21" t="s">
         <v>48</v>
       </c>
+      <c r="D21" t="s">
+        <v>160</v>
+      </c>
       <c r="E21" t="s">
         <v>54</v>
       </c>
@@ -1168,6 +1333,9 @@
       <c r="C22" t="s">
         <v>48</v>
       </c>
+      <c r="D22" t="s">
+        <v>152</v>
+      </c>
       <c r="E22" t="s">
         <v>54</v>
       </c>
@@ -1185,6 +1353,9 @@
       <c r="C23" t="s">
         <v>48</v>
       </c>
+      <c r="D23" t="s">
+        <v>151</v>
+      </c>
       <c r="E23" t="s">
         <v>54</v>
       </c>
@@ -1202,6 +1373,9 @@
       <c r="C24" t="s">
         <v>48</v>
       </c>
+      <c r="D24" t="s">
+        <v>159</v>
+      </c>
       <c r="E24" t="s">
         <v>54</v>
       </c>
@@ -1219,6 +1393,9 @@
       <c r="C25" t="s">
         <v>48</v>
       </c>
+      <c r="D25" t="s">
+        <v>158</v>
+      </c>
       <c r="E25" t="s">
         <v>54</v>
       </c>
@@ -1236,6 +1413,9 @@
       <c r="C26" t="s">
         <v>48</v>
       </c>
+      <c r="D26" t="s">
+        <v>157</v>
+      </c>
       <c r="E26" t="s">
         <v>54</v>
       </c>
@@ -1253,6 +1433,9 @@
       <c r="C27" t="s">
         <v>48</v>
       </c>
+      <c r="D27" t="s">
+        <v>156</v>
+      </c>
       <c r="E27" t="s">
         <v>54</v>
       </c>
@@ -1270,6 +1453,9 @@
       <c r="C28" t="s">
         <v>48</v>
       </c>
+      <c r="D28" t="s">
+        <v>147</v>
+      </c>
       <c r="E28" t="s">
         <v>55</v>
       </c>
@@ -1287,6 +1473,9 @@
       <c r="C29" t="s">
         <v>48</v>
       </c>
+      <c r="D29" t="s">
+        <v>146</v>
+      </c>
       <c r="E29" t="s">
         <v>55</v>
       </c>
@@ -1304,6 +1493,9 @@
       <c r="C30" t="s">
         <v>48</v>
       </c>
+      <c r="D30" t="s">
+        <v>148</v>
+      </c>
       <c r="E30" t="s">
         <v>55</v>
       </c>
@@ -1321,6 +1513,9 @@
       <c r="C31" t="s">
         <v>48</v>
       </c>
+      <c r="D31" t="s">
+        <v>149</v>
+      </c>
       <c r="E31" t="s">
         <v>55</v>
       </c>
@@ -1338,6 +1533,9 @@
       <c r="C32" t="s">
         <v>48</v>
       </c>
+      <c r="D32" t="s">
+        <v>150</v>
+      </c>
       <c r="E32" t="s">
         <v>55</v>
       </c>
@@ -1355,6 +1553,9 @@
       <c r="C33" t="s">
         <v>44</v>
       </c>
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
       <c r="E33" t="s">
         <v>52</v>
       </c>
@@ -1423,6 +1624,9 @@
       <c r="C37" t="s">
         <v>49</v>
       </c>
+      <c r="D37" t="s">
+        <v>163</v>
+      </c>
       <c r="E37" t="s">
         <v>53</v>
       </c>
@@ -1440,6 +1644,9 @@
       <c r="C38" t="s">
         <v>49</v>
       </c>
+      <c r="D38" t="s">
+        <v>163</v>
+      </c>
       <c r="E38" t="s">
         <v>53</v>
       </c>
@@ -1457,6 +1664,9 @@
       <c r="C39" t="s">
         <v>49</v>
       </c>
+      <c r="D39" t="s">
+        <v>163</v>
+      </c>
       <c r="E39" t="s">
         <v>53</v>
       </c>
@@ -1474,6 +1684,9 @@
       <c r="C40" t="s">
         <v>49</v>
       </c>
+      <c r="D40" t="s">
+        <v>163</v>
+      </c>
       <c r="E40" t="s">
         <v>53</v>
       </c>
@@ -1491,6 +1704,9 @@
       <c r="C41" t="s">
         <v>49</v>
       </c>
+      <c r="D41" t="s">
+        <v>163</v>
+      </c>
       <c r="E41" t="s">
         <v>53</v>
       </c>
@@ -1525,6 +1741,9 @@
       <c r="C43" t="s">
         <v>50</v>
       </c>
+      <c r="D43" t="s">
+        <v>138</v>
+      </c>
       <c r="E43" t="s">
         <v>94</v>
       </c>
@@ -1540,7 +1759,13 @@
         <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" t="s">
+        <v>120</v>
       </c>
       <c r="F44">
         <v>2013</v>
@@ -1554,7 +1779,13 @@
         <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D45" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" t="s">
+        <v>120</v>
       </c>
       <c r="F45">
         <v>2013</v>
@@ -1568,7 +1799,13 @@
         <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D46" t="s">
+        <v>128</v>
+      </c>
+      <c r="E46" t="s">
+        <v>120</v>
       </c>
       <c r="F46">
         <v>2013</v>
@@ -1582,7 +1819,13 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" t="s">
+        <v>120</v>
       </c>
       <c r="F47">
         <v>2013</v>
@@ -1596,7 +1839,13 @@
         <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D48" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" t="s">
+        <v>120</v>
       </c>
       <c r="F48">
         <v>2013</v>
@@ -1610,7 +1859,13 @@
         <v>70</v>
       </c>
       <c r="C49" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D49" t="s">
+        <v>129</v>
+      </c>
+      <c r="E49" t="s">
+        <v>120</v>
       </c>
       <c r="F49">
         <v>2013</v>
@@ -1624,7 +1879,13 @@
         <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D50" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" t="s">
+        <v>120</v>
       </c>
       <c r="F50">
         <v>2013</v>
@@ -1638,7 +1899,13 @@
         <v>72</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D51" t="s">
+        <v>131</v>
+      </c>
+      <c r="E51" t="s">
+        <v>120</v>
       </c>
       <c r="F51">
         <v>2013</v>
@@ -1652,7 +1919,13 @@
         <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D52" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" t="s">
+        <v>120</v>
       </c>
       <c r="F52">
         <v>2013</v>
@@ -1666,7 +1939,13 @@
         <v>74</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D53" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" t="s">
+        <v>120</v>
       </c>
       <c r="F53">
         <v>2013</v>
@@ -1680,7 +1959,13 @@
         <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D54" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" t="s">
+        <v>120</v>
       </c>
       <c r="F54">
         <v>2013</v>
@@ -1694,7 +1979,13 @@
         <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D55" t="s">
+        <v>123</v>
+      </c>
+      <c r="E55" t="s">
+        <v>120</v>
       </c>
       <c r="F55">
         <v>2013</v>
@@ -1708,7 +1999,13 @@
         <v>77</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D56" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" t="s">
+        <v>120</v>
       </c>
       <c r="F56">
         <v>2013</v>
@@ -1722,7 +2019,13 @@
         <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D57" t="s">
+        <v>135</v>
+      </c>
+      <c r="E57" t="s">
+        <v>120</v>
       </c>
       <c r="F57">
         <v>2013</v>
@@ -1736,7 +2039,13 @@
         <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D58" t="s">
+        <v>136</v>
+      </c>
+      <c r="E58" t="s">
+        <v>120</v>
       </c>
       <c r="F58">
         <v>2013</v>
@@ -1750,7 +2059,13 @@
         <v>80</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>121</v>
+      </c>
+      <c r="D59" t="s">
+        <v>137</v>
+      </c>
+      <c r="E59" t="s">
+        <v>120</v>
       </c>
       <c r="F59">
         <v>2013</v>
@@ -1758,24 +2073,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3AEA1D-A8EC-46B4-BE03-641E1C2925B7}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -1785,8 +2101,11 @@
       <c r="C1" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1794,7 +2113,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1802,7 +2121,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1810,15 +2129,21 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1827,6 +2152,14 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1837,8 +2170,11 @@
     <hyperlink ref="B4" r:id="rId4" xr:uid="{2AD6C0E9-2474-4DA8-95D2-9CA0C8385359}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{977751B1-EA9A-4549-B042-3A70513220BD}"/>
     <hyperlink ref="C6" r:id="rId6" location="disclaimers " xr:uid="{5CC2D0CA-0268-4E6B-88D4-AD1CD49C12DD}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{3BC5096D-C9DD-48D1-948E-40D15F44B471}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{9F5D0360-8ECF-4E3C-98F7-8989409FA611}"/>
+    <hyperlink ref="D5" r:id="rId9" xr:uid="{BCC163C0-6B7A-4C0C-B99B-6894A694C299}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final edits to prac 3 and update to metadata
</commit_message>
<xml_diff>
--- a/Data/LSOA_metadata.xlsx
+++ b/Data/LSOA_metadata.xlsx
@@ -141,9 +141,6 @@
     <t>Persons per household</t>
   </si>
   <si>
-    <t>Persons per ??</t>
-  </si>
-  <si>
     <t>https://www.ordnancesurvey.co.uk/business-and-government/products/vectormap-district.html</t>
   </si>
   <si>
@@ -451,6 +448,9 @@
   </si>
   <si>
     <t>Accomodation type</t>
+  </si>
+  <si>
+    <t>Persons per hectare</t>
   </si>
 </sst>
 </file>
@@ -825,7 +825,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
         <v>36</v>
@@ -878,7 +878,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
@@ -895,7 +895,7 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>36</v>
@@ -912,7 +912,7 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
@@ -929,7 +929,7 @@
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>36</v>
@@ -946,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
@@ -963,7 +963,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
         <v>36</v>
@@ -980,7 +980,7 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -997,7 +997,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -1014,7 +1014,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
@@ -1031,7 +1031,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
@@ -1048,10 +1048,10 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>141</v>
       </c>
       <c r="E13">
         <v>2011</v>
@@ -1065,7 +1065,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -1082,7 +1082,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
@@ -1099,7 +1099,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -1119,7 +1119,7 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17">
         <v>2017</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1136,7 +1136,7 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <v>2017</v>
@@ -1150,7 +1150,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
@@ -1161,13 +1161,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
@@ -1178,13 +1178,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" t="s">
         <v>33</v>
@@ -1195,13 +1195,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D22" t="s">
         <v>33</v>
@@ -1212,13 +1212,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D23" t="s">
         <v>33</v>
@@ -1229,13 +1229,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
@@ -1246,13 +1246,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D25" t="s">
         <v>33</v>
@@ -1263,13 +1263,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" t="s">
         <v>33</v>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27" t="s">
         <v>33</v>
@@ -1303,7 +1303,7 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D28" t="s">
         <v>34</v>
@@ -1314,13 +1314,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
         <v>34</v>
@@ -1331,13 +1331,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
@@ -1348,13 +1348,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" t="s">
         <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D31" t="s">
         <v>34</v>
@@ -1365,13 +1365,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
         <v>23</v>
@@ -1399,13 +1399,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
         <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E34">
         <v>2017</v>
@@ -1413,13 +1413,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
         <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E35">
         <v>2017</v>
@@ -1427,13 +1427,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
         <v>28</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E36">
         <v>2017</v>
@@ -1441,13 +1441,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D37" t="s">
         <v>32</v>
@@ -1458,13 +1458,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
         <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D38" t="s">
         <v>32</v>
@@ -1475,13 +1475,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s">
         <v>32</v>
@@ -1492,13 +1492,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
         <v>28</v>
       </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s">
         <v>32</v>
@@ -1509,13 +1509,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D41" t="s">
         <v>32</v>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
@@ -1546,10 +1546,10 @@
         <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E43">
         <v>2011</v>
@@ -1557,16 +1557,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E44">
         <v>2013</v>
@@ -1574,16 +1574,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E45">
         <v>2013</v>
@@ -1591,16 +1591,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E46">
         <v>2013</v>
@@ -1608,16 +1608,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
         <v>99</v>
       </c>
-      <c r="C47" t="s">
-        <v>100</v>
-      </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E47">
         <v>2013</v>
@@ -1625,16 +1625,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E48">
         <v>2013</v>
@@ -1642,16 +1642,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E49">
         <v>2013</v>
@@ -1659,16 +1659,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E50">
         <v>2013</v>
@@ -1676,16 +1676,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E51">
         <v>2013</v>
@@ -1693,16 +1693,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E52">
         <v>2013</v>
@@ -1710,16 +1710,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E53">
         <v>2013</v>
@@ -1727,16 +1727,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E54">
         <v>2013</v>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E55">
         <v>2013</v>
@@ -1761,16 +1761,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C56" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E56">
         <v>2013</v>
@@ -1778,16 +1778,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E57">
         <v>2013</v>
@@ -1795,16 +1795,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E58">
         <v>2013</v>
@@ -1812,16 +1812,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E59">
         <v>2013</v>
@@ -1852,13 +1852,13 @@
         <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1874,7 +1874,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,7 +1882,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,13 +1890,13 @@
         <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,18 +1904,18 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>